<commit_message>
Se crea pagina de Campañas y se configura los colores del status
</commit_message>
<xml_diff>
--- a/Server/src/db/DB Inicial.xlsx
+++ b/Server/src/db/DB Inicial.xlsx
@@ -5,11 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DB_ETN" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="DB_GHO" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Campañas ETN" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="Campañas GHO" sheetId="4" state="visible" r:id="rId6"/>
+    <sheet name="Campañas Cotaline" sheetId="5" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">DB_ETN!$A$1:$D$57</definedName>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="163">
   <si>
     <t xml:space="preserve">nombre</t>
   </si>
@@ -316,14 +319,213 @@
   </si>
   <si>
     <t xml:space="preserve">Zamora Plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha_inicio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fecha_fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aviso de privacidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OLWAYS ON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALTA ACTUALIZAR ARTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abordaje he identificación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Términos y condiciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aviso de no discriminación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aviso migratorio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viaje redondo 10 + 15 APP y WEB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACTIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25% + 5% de descuento (venta anticipada RM) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARTES SIN ENTREGAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra aquí tu boleto Viva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiventa Costaline y Autovias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiventa Almealsences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seguro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multienvios</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Descuentos de temporada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinturón de seguridad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suburbano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pay Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta Los Mochis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Escalas Puebla - Monterrey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeropuerto AICM (Poninte Uruapan-Morelia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeropuerto AICM Quere-SanMiguel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeropuerto AIFA (Qto, SJD)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeropuerto AIFA con Viva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta Norte - Papagayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta CDMX – Tepochutla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desc INAPAM - PCD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INACTIVA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Medidas de control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No discriminacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abordaje he Identificacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminos y condiciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doters Boleto Recompensa y Usa puntos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paypal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web y app 10 + 15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiventa - ETN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Viva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enlace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiventa Amealcenses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rutas de San Felipe a (jilotepec, Metro,Rosario, MexNorte, Tepotzotlan)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta de poninete a (Zitacuaro GDL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta MEXN-GDL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HP (Toluca - Morelia)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morelia - Ixtapa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autobuses Nuevos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta GDL a Colima Manzanillo CDGUZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desc Temporada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abordaje Identificacion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aviso de Privacidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Costapass</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compra anticipada 35 + 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Doters </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiventa ETN  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiventa ETN y Autovias</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boleto Electronico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rutas Taxqueña</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEXS-PPG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Promo Norte - Papagayo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ruta CDMX - Tepochutla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rutas Zihuatanejo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des Temp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -410,7 +612,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -423,7 +625,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -704,7 +918,7 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1532,14 +1746,14 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1557,479 +1771,479 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="0" t="s">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="C3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="0" t="s">
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="0" t="s">
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="0" t="s">
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="0" t="s">
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="0" t="s">
+      <c r="C10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="0" t="s">
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="0" t="s">
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="0" t="s">
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="0" t="s">
+      <c r="C15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="0" t="s">
+      <c r="C16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="C17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="0" t="s">
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="0" t="s">
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="0" t="s">
+      <c r="C20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="B21" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="0" t="s">
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D22" s="0" t="s">
+      <c r="B22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="0" t="s">
+      <c r="C23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B24" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="0" t="s">
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="0" t="s">
+      <c r="C25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C26" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D26" s="0" t="s">
+      <c r="B26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C27" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="0" t="s">
+      <c r="B27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="B28" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C28" s="0" t="s">
+      <c r="B28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="0" t="s">
+      <c r="D28" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="0" t="s">
+      <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D30" s="0" t="s">
+      <c r="B30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C31" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="0" t="s">
+      <c r="C31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D32" s="0" t="s">
+      <c r="B32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="0" t="s">
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D34" s="0" t="s">
+      <c r="B34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" s="0" t="s">
+      <c r="B35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="1" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2044,4 +2258,1061 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D27"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="29.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="61.26"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B24" s="6" t="n">
+        <v>45393</v>
+      </c>
+      <c r="C24" s="6" t="n">
+        <v>45390</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.9"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D16" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;KffffffPágina &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>